<commit_message>
Corrected spelling on Cider listings
As raised by Claire
</commit_message>
<xml_diff>
--- a/listings/cider.xlsx
+++ b/listings/cider.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmagu\OneDrive\Documents\Beer Festival 2017\Website\1 - cbcf.info\listings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F4F83637-DDA6-4436-A484-45FF6DC8D331}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23955" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -262,9 +271,6 @@
     <t>Farmer Jim's</t>
   </si>
   <si>
-    <t>Torquay, devon</t>
-  </si>
-  <si>
     <t>Vintage Garden Cider Medium</t>
   </si>
   <si>
@@ -584,77 +590,388 @@
   </si>
   <si>
     <t>Wells-next-the-Sea, Norfolk</t>
+  </si>
+  <si>
+    <t>Torquay, Devon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.29"/>
-    <col customWidth="1" min="2" max="2" width="20.71"/>
-    <col customWidth="1" min="3" max="3" width="27.71"/>
-    <col customWidth="1" min="4" max="4" width="7.0"/>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -679,10 +996,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="2">
-        <v>4.6</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -696,7 +1013,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -710,7 +1027,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -724,7 +1041,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -735,10 +1052,10 @@
         <v>6</v>
       </c>
       <c r="D6" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -752,7 +1069,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -766,7 +1083,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -780,7 +1097,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -794,7 +1111,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -808,7 +1125,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -819,10 +1136,10 @@
         <v>16</v>
       </c>
       <c r="D12" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -833,10 +1150,10 @@
         <v>16</v>
       </c>
       <c r="D13" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -850,7 +1167,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -861,10 +1178,10 @@
         <v>16</v>
       </c>
       <c r="D15" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -878,7 +1195,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -892,7 +1209,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -906,7 +1223,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -917,10 +1234,10 @@
         <v>27</v>
       </c>
       <c r="D19" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
@@ -931,10 +1248,10 @@
         <v>27</v>
       </c>
       <c r="D20" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -948,7 +1265,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -959,10 +1276,10 @@
         <v>34</v>
       </c>
       <c r="D22" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
@@ -973,10 +1290,10 @@
         <v>34</v>
       </c>
       <c r="D23" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
@@ -987,10 +1304,10 @@
         <v>34</v>
       </c>
       <c r="D24" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
@@ -1001,10 +1318,10 @@
         <v>34</v>
       </c>
       <c r="D25" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -1015,10 +1332,10 @@
         <v>34</v>
       </c>
       <c r="D26" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
@@ -1032,7 +1349,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>42</v>
       </c>
@@ -1046,7 +1363,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
@@ -1057,10 +1374,10 @@
         <v>47</v>
       </c>
       <c r="D29" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
@@ -1074,7 +1391,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>49</v>
       </c>
@@ -1088,7 +1405,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>50</v>
       </c>
@@ -1099,10 +1416,10 @@
         <v>47</v>
       </c>
       <c r="D32" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -1113,10 +1430,10 @@
         <v>47</v>
       </c>
       <c r="D33" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>52</v>
       </c>
@@ -1127,10 +1444,10 @@
         <v>54</v>
       </c>
       <c r="D34" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>55</v>
       </c>
@@ -1141,10 +1458,10 @@
         <v>57</v>
       </c>
       <c r="D35" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>58</v>
       </c>
@@ -1158,7 +1475,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>61</v>
       </c>
@@ -1169,10 +1486,10 @@
         <v>60</v>
       </c>
       <c r="D37" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>62</v>
       </c>
@@ -1186,7 +1503,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>63</v>
       </c>
@@ -1200,7 +1517,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>64</v>
       </c>
@@ -1211,10 +1528,10 @@
         <v>66</v>
       </c>
       <c r="D40" s="2">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>67</v>
       </c>
@@ -1225,10 +1542,10 @@
         <v>66</v>
       </c>
       <c r="D41" s="2">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>68</v>
       </c>
@@ -1239,10 +1556,10 @@
         <v>66</v>
       </c>
       <c r="D42" s="2">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>69</v>
       </c>
@@ -1253,10 +1570,10 @@
         <v>71</v>
       </c>
       <c r="D43" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>72</v>
       </c>
@@ -1270,7 +1587,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>75</v>
       </c>
@@ -1284,7 +1601,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>76</v>
       </c>
@@ -1298,7 +1615,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>77</v>
       </c>
@@ -1312,7 +1629,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>80</v>
       </c>
@@ -1326,7 +1643,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>81</v>
       </c>
@@ -1334,986 +1651,985 @@
         <v>82</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D49" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D49" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D50" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D51" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D52" s="2">
         <v>7.5</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D53" s="2">
         <v>7.5</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D54" s="2">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="B55" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="D55" s="2">
         <v>4.5</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="D56" s="2">
         <v>7.2</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D57" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="D58" s="2">
         <v>4.5</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="D59" s="2">
         <v>4.5</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D60" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="2" t="s">
+      <c r="B61" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D61" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D61" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="D62" s="2">
         <v>6.2</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D63" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D63" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="D64" s="2">
         <v>6.2</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="D65" s="2">
         <v>4.5</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D66" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D66" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="D67" s="2">
         <v>5.5</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="D68" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="69">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="D69" s="2">
         <v>5.5</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D70" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="B71" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="D71" s="2">
         <v>5.5</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="D72" s="2">
         <v>5.5</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="D73" s="2">
         <v>5.5</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="C74" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D74" s="2">
         <v>6.5</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D75" s="2">
         <v>5.5</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D76" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="B77" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D77" s="2">
         <v>5.2</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D78" s="2">
         <v>7.5</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D79" s="2">
         <v>6.8</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D80" s="2">
         <v>7.5</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D81" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D81" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="2" t="s">
+      <c r="D82" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D82" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="2" t="s">
+      <c r="D83" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D84" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B85" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D83" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D84" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D85" s="2">
         <v>7.5</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="D86" s="2">
         <v>5.5</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="D87" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D87" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="2" t="s">
+      <c r="B88" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D88" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D88" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="D89" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D89" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="2" t="s">
+      <c r="B90" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D90" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D90" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="D91" s="2">
         <v>4.5</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="D92" s="2">
         <v>3.8</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D93" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D93" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="2" t="s">
+      <c r="D94" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D94" s="2">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="2" t="s">
+      <c r="D95" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D95" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="2" t="s">
+      <c r="D96" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D96" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="D97" s="2">
         <v>5.3</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="D98" s="2">
         <v>5.2</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="D99" s="2">
-        <v>4.6</v>
-      </c>
-    </row>
-    <row r="100">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="D100" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D100" s="2">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="D101" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D101" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="D102" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D102" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="D103" s="2">
         <v>5.5</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="D104" s="2">
         <v>7.2</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="D105" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D106" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D105" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D106" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="D107" s="2">
         <v>3.5</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D108" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B109" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D108" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="D109" s="2">
         <v>3.8</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B110" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="D110" s="2">
         <v>5.8</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="D111" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D111" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D112" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="113">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D113" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="114">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="D114" s="2">
         <v>4.5</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D115" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D115" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="D116" s="2">
         <v>6.5</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>190</v>
       </c>
       <c r="D117" s="2">
         <v>5.8</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B118" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C118" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>190</v>
       </c>
       <c r="D118" s="2">
         <v>5.4</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
   <headerFooter>
     <oddHeader>&amp;LChelmsford Summer Beer &amp;&amp; Cider Festival 2018&amp;RCider Listing</oddHeader>
     <oddFooter>&amp;LLast updated 30/06/2018&amp;Rwww.cbcf.info/cider</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>